<commit_message>
Updated use cases doc
</commit_message>
<xml_diff>
--- a/design/use cases.xlsx
+++ b/design/use cases.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="49">
   <si>
     <t>use case</t>
   </si>
@@ -26,22 +26,113 @@
     <t>pre-condition</t>
   </si>
   <si>
+    <t>use case 0</t>
+  </si>
+  <si>
+    <t>initial display</t>
+  </si>
+  <si>
+    <t>response</t>
+  </si>
+  <si>
     <t>components</t>
   </si>
   <si>
+    <t>models</t>
+  </si>
+  <si>
     <t>message title textfield</t>
   </si>
   <si>
+    <t>user logs in</t>
+  </si>
+  <si>
+    <t>user</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+      </rPr>
+      <t>constituent</t>
+    </r>
+    <r>
+      <t xml:space="preserve"> communicates expectations </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+      </rPr>
+      <t>to official</t>
+    </r>
+  </si>
+  <si>
+    <t>text display/label</t>
+  </si>
+  <si>
+    <t>user specifies expectation</t>
+  </si>
+  <si>
     <t>officials have been created in the system</t>
   </si>
   <si>
+    <t>constituency</t>
+  </si>
+  <si>
+    <t>message box or textarea</t>
+  </si>
+  <si>
+    <t>save button</t>
+  </si>
+  <si>
     <t>users can register in the system as constituents</t>
   </si>
   <si>
-    <t>use case 0</t>
-  </si>
-  <si>
-    <t>message box or textarea</t>
+    <t>send button</t>
+  </si>
+  <si>
+    <t>office select</t>
+  </si>
+  <si>
+    <t>office</t>
+  </si>
+  <si>
+    <t>official</t>
+  </si>
+  <si>
+    <t>official select</t>
+  </si>
+  <si>
+    <t>constituent communicates expectations to office</t>
+  </si>
+  <si>
+    <t>user selects office</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+      </rPr>
+      <t>statutory duties</t>
+    </r>
+    <r>
+      <t xml:space="preserve"> populated into system as </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+      </rPr>
+      <t>expectations</t>
+    </r>
+  </si>
+  <si>
+    <t>pollingUnit</t>
+  </si>
+  <si>
+    <t>local council</t>
+  </si>
+  <si>
+    <t>councillor</t>
   </si>
   <si>
     <r>
@@ -51,6 +142,34 @@
       <t>constituent</t>
     </r>
     <r>
+      <t xml:space="preserve"> chooses </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+      </rPr>
+      <t>candidate</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+      </rPr>
+      <t>delineation of duties</t>
+    </r>
+    <r>
+      <t xml:space="preserve"> of each office from local to federal has been done within system</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+      </rPr>
+      <t>constituent</t>
+    </r>
+    <r>
       <t xml:space="preserve"> communicates expectations </t>
     </r>
     <r>
@@ -61,20 +180,32 @@
     </r>
   </si>
   <si>
-    <t>save button</t>
-  </si>
-  <si>
-    <t>send button</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-      </rPr>
-      <t>statutory duties</t>
-    </r>
-    <r>
-      <t xml:space="preserve"> populated into system as </t>
+    <t>candidates displayed horizontally</t>
+  </si>
+  <si>
+    <t>user selects official</t>
+  </si>
+  <si>
+    <t>ward</t>
+  </si>
+  <si>
+    <t>each candidate details can be scrolled through</t>
+  </si>
+  <si>
+    <t>ability to click candidate to select</t>
+  </si>
+  <si>
+    <t>user submits request</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+      </rPr>
+      <t>manifesto</t>
+    </r>
+    <r>
+      <t xml:space="preserve"> has been populated in system as </t>
     </r>
     <r>
       <rPr>
@@ -84,31 +215,14 @@
     </r>
   </si>
   <si>
-    <t>office select</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-      </rPr>
-      <t>delineation of duties</t>
-    </r>
-    <r>
-      <t xml:space="preserve"> of each office from local to federal has been done within system</t>
-    </r>
-  </si>
-  <si>
-    <t>official select</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-      </rPr>
-      <t>manifesto</t>
-    </r>
-    <r>
-      <t xml:space="preserve"> has been populated in system as </t>
+    <r>
+      <rPr>
+        <b/>
+      </rPr>
+      <t xml:space="preserve">campaign promises </t>
+    </r>
+    <r>
+      <t xml:space="preserve">have been populated into system as </t>
     </r>
     <r>
       <rPr>
@@ -122,10 +236,10 @@
       <rPr>
         <b/>
       </rPr>
-      <t xml:space="preserve">campaign promises </t>
-    </r>
-    <r>
-      <t xml:space="preserve">have been populated into system as </t>
+      <t>current budget projects</t>
+    </r>
+    <r>
+      <t xml:space="preserve"> have been populated into system as </t>
     </r>
     <r>
       <rPr>
@@ -135,23 +249,6 @@
     </r>
   </si>
   <si>
-    <r>
-      <rPr>
-        <b/>
-      </rPr>
-      <t>current budget projects</t>
-    </r>
-    <r>
-      <t xml:space="preserve"> have been populated into system as </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-      </rPr>
-      <t>expectations</t>
-    </r>
-  </si>
-  <si>
     <t>use case 1</t>
   </si>
   <si>
@@ -168,70 +265,11 @@
       <rPr>
         <b/>
       </rPr>
-      <t>officials</t>
-    </r>
-  </si>
-  <si>
-    <t>models</t>
-  </si>
-  <si>
-    <t>user logs in</t>
-  </si>
-  <si>
-    <t>user</t>
-  </si>
-  <si>
-    <t>user specifies expectation</t>
-  </si>
-  <si>
-    <t>constituency</t>
-  </si>
-  <si>
-    <t>office</t>
-  </si>
-  <si>
-    <t>official</t>
-  </si>
-  <si>
-    <t>constituent communicates expectations to office</t>
-  </si>
-  <si>
-    <t>user selects office</t>
-  </si>
-  <si>
-    <t>pollingUnit</t>
-  </si>
-  <si>
-    <t>local council</t>
-  </si>
-  <si>
-    <t>councillor</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-      </rPr>
-      <t>constituent</t>
-    </r>
-    <r>
-      <t xml:space="preserve"> communicates expectations </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-      </rPr>
-      <t>to official</t>
-    </r>
-  </si>
-  <si>
-    <t>user selects official</t>
-  </si>
-  <si>
-    <t>ward</t>
-  </si>
-  <si>
-    <t>user submits request</t>
+      <t>candidate</t>
+    </r>
+  </si>
+  <si>
+    <t>candidates have been created in the system</t>
   </si>
   <si>
     <t>technical</t>
@@ -355,15 +393,15 @@
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1" t="s">
-        <v>21</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2">
       <c r="B2" s="2" t="s">
-        <v>22</v>
+        <v>9</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>23</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3">
@@ -371,38 +409,38 @@
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>24</v>
+        <v>13</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D4" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="E4" s="2" t="s">
         <v>29</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>34</v>
@@ -414,7 +452,7 @@
     <row r="6">
       <c r="A6" s="2"/>
       <c r="B6" s="2" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C6" s="3"/>
     </row>
@@ -450,45 +488,78 @@
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <cols>
     <col customWidth="1" min="1" max="1" width="33.57"/>
-    <col customWidth="1" min="2" max="2" width="22.86"/>
+    <col customWidth="1" min="2" max="2" width="39.43"/>
+    <col customWidth="1" min="3" max="3" width="14.86"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
+      <c r="B1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>4</v>
+        <v>8</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="3">
       <c r="B3" s="1" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4">
       <c r="B4" s="3" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5">
       <c r="B5" s="1" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6">
       <c r="B6" s="3" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7">
       <c r="B7" s="3" t="s">
-        <v>15</v>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="B10" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="B11" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="B12" s="2" t="s">
+        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -521,56 +592,67 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="2"/>
-      <c r="B2" s="2"/>
+      <c r="A2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>11</v>
+      </c>
       <c r="C2" s="2" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="2"/>
       <c r="B3" s="2"/>
       <c r="C3" s="2" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>9</v>
-      </c>
       <c r="C4" s="2" t="s">
-        <v>12</v>
+        <v>26</v>
       </c>
     </row>
     <row r="5">
       <c r="C5" s="2" t="s">
-        <v>14</v>
+        <v>31</v>
       </c>
     </row>
     <row r="6">
       <c r="C6" s="2" t="s">
-        <v>16</v>
+        <v>39</v>
       </c>
     </row>
     <row r="7">
       <c r="C7" s="2" t="s">
-        <v>17</v>
+        <v>40</v>
       </c>
     </row>
     <row r="8">
       <c r="C8" s="2" t="s">
-        <v>18</v>
+        <v>41</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="2" t="s">
-        <v>19</v>
+        <v>42</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>20</v>
+        <v>43</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="C11" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="C12" s="2" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -593,35 +675,35 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="2" t="s">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="2" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>38</v>
+        <v>46</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="s">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -641,7 +723,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="2" t="s">
-        <v>37</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>